<commit_message>
Events Updated, with profile & Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="201">
   <si>
     <t>Subject Code</t>
   </si>
@@ -595,6 +595,36 @@
   </si>
   <si>
     <t>wqe</t>
+  </si>
+  <si>
+    <t>2345789</t>
+  </si>
+  <si>
+    <t>sdwdd</t>
+  </si>
+  <si>
+    <t>dedeedd</t>
+  </si>
+  <si>
+    <t>ded</t>
+  </si>
+  <si>
+    <t>eded</t>
+  </si>
+  <si>
+    <t>Paid ($1000.0)</t>
+  </si>
+  <si>
+    <t>dede</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>10/5/2025 14:00</t>
+  </si>
+  <si>
+    <t>Paid ($20.0)</t>
   </si>
 </sst>
 </file>
@@ -8940,7 +8970,7 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9017,34 +9047,64 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="E3" s="6">
-        <v>45935.583333333336</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="E4" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="F4" t="n" s="0">
         <v>50.0</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="G4" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
+      <c r="I4" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -10024,7 +10084,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
excel stores student info
</commit_message>
<xml_diff>
--- a/src/main/resources/UMS_Data.xlsx
+++ b/src/main/resources/UMS_Data.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azahi\OneDrive - University of Guelph\1st Year\Semester 2\University-Management\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817D889-0505-4B9D-9AE6-1EB7E16E98E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7075D-F510-4AC9-985B-9783054BC5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
     <sheet name="Courses" sheetId="2" r:id="rId2"/>
-    <sheet name="Students " sheetId="3" r:id="rId3"/>
-    <sheet name="Faculties " sheetId="4" r:id="rId4"/>
-    <sheet name="Events " sheetId="5" r:id="rId5"/>
+    <sheet name="Students" sheetId="3" r:id="rId3"/>
+    <sheet name="Faculties" sheetId="4" r:id="rId4"/>
+    <sheet name="Events" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="198">
   <si>
     <t>Subject Code</t>
   </si>
@@ -277,9 +277,6 @@
     <t>S20250002</t>
   </si>
   <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
     <t>456 Oak St.</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>S20250008</t>
   </si>
   <si>
-    <t>Helen Jones</t>
-  </si>
-  <si>
     <t>333 Maple Dr.</t>
   </si>
   <si>
@@ -574,34 +568,61 @@
     <t>Lab 301</t>
   </si>
   <si>
-    <t>2345789</t>
-  </si>
-  <si>
-    <t>sdwdd</t>
-  </si>
-  <si>
-    <t>dedeedd</t>
-  </si>
-  <si>
-    <t>ded</t>
-  </si>
-  <si>
-    <t>eded</t>
-  </si>
-  <si>
-    <t>Paid ($1000.0)</t>
-  </si>
-  <si>
-    <t>dede</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>10/5/2025 14:00</t>
-  </si>
-  <si>
-    <t>Paid ($20.0)</t>
+    <t>Paid ($20)</t>
+  </si>
+  <si>
+    <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>Bob Johnsoners</t>
+  </si>
+  <si>
+    <t>S20250011</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Helen Jonesed</t>
+  </si>
+  <si>
+    <t>adfd</t>
+  </si>
+  <si>
+    <t>nigga</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Alice Smithserfgd</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>dfrs</t>
+  </si>
+  <si>
+    <t>Alice Smithser</t>
+  </si>
+  <si>
+    <t>Carol Williamses</t>
+  </si>
+  <si>
+    <t>Alice Smithsersd</t>
+  </si>
+  <si>
+    <t>esf</t>
+  </si>
+  <si>
+    <t>Bob Johnsonerses</t>
+  </si>
+  <si>
+    <t>CS201,BIO300</t>
   </si>
 </sst>
 </file>
@@ -612,7 +633,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ h:mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +676,11 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -921,9 +947,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="26" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="2" max="2" customWidth="true" width="25.5703125"/>
+    <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -4980,16 +5006,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="26" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.28515625"/>
+    <col min="2" max="2" customWidth="true" width="27.0"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375"/>
+    <col min="4" max="4" customWidth="true" width="15.42578125"/>
+    <col min="5" max="5" customWidth="true" width="8.7109375"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875"/>
+    <col min="7" max="7" customWidth="true" width="20.5703125"/>
+    <col min="8" max="8" customWidth="true" width="9.5703125"/>
+    <col min="9" max="9" customWidth="true" width="16.5703125"/>
+    <col min="10" max="26" customWidth="true" width="10.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,26 +6334,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="72.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="26" width="10" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.0"/>
+    <col min="2" max="2" customWidth="true" width="14.140625"/>
+    <col min="3" max="3" customWidth="true" width="12.42578125"/>
+    <col min="4" max="4" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125"/>
+    <col min="7" max="7" customWidth="true" width="16.0"/>
+    <col min="8" max="8" customWidth="true" width="12.28515625"/>
+    <col min="9" max="9" customWidth="true" width="26.85546875"/>
+    <col min="10" max="10" customWidth="true" width="72.140625"/>
+    <col min="11" max="11" customWidth="true" width="8.7109375"/>
+    <col min="12" max="26" customWidth="true" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6373,7 +6399,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>194</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>73</v>
@@ -6399,8 +6425,8 @@
       <c r="J2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="10">
-        <v>0.4</v>
+      <c r="K2" s="10" t="s">
+        <v>190</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>80</v>
@@ -6411,19 +6437,19 @@
         <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>77</v>
@@ -6432,13 +6458,13 @@
         <v>78</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>6</v>
+        <v>197</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0.5</v>
+        <v>86</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>80</v>
@@ -6446,22 +6472,22 @@
     </row>
     <row r="4" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>77</v>
@@ -6470,13 +6496,13 @@
         <v>78</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.5</v>
+      <c r="K4" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>80</v>
@@ -6484,19 +6510,19 @@
     </row>
     <row r="5" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>76</v>
@@ -6508,7 +6534,7 @@
         <v>78</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>79</v>
@@ -6522,19 +6548,19 @@
     </row>
     <row r="6" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>76</v>
@@ -6549,7 +6575,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K6" s="13">
         <v>0.5</v>
@@ -6560,22 +6586,22 @@
     </row>
     <row r="7" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>77</v>
@@ -6584,10 +6610,10 @@
         <v>78</v>
       </c>
       <c r="I7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="K7" s="13">
         <v>0.5</v>
@@ -6598,19 +6624,19 @@
     </row>
     <row r="8" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>76</v>
@@ -6622,13 +6648,13 @@
         <v>78</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" s="13">
-        <v>0.4</v>
+        <v>105</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>80</v>
@@ -6636,22 +6662,22 @@
     </row>
     <row r="9" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>77</v>
@@ -6660,13 +6686,13 @@
         <v>78</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K9" s="13">
-        <v>0.5</v>
+        <v>124</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>80</v>
@@ -6674,19 +6700,19 @@
     </row>
     <row r="10" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>76</v>
@@ -6698,7 +6724,7 @@
         <v>78</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>79</v>
@@ -6712,22 +6738,22 @@
     </row>
     <row r="11" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>77</v>
@@ -6739,7 +6765,7 @@
         <v>14</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K11" s="13">
         <v>0.2</v>
@@ -6748,7 +6774,44 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7737,7 +7800,9 @@
     <row r="998" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
@@ -7754,38 +7819,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="26" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="8.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.42578125"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625"/>
+    <col min="7" max="7" customWidth="true" width="20.0"/>
+    <col min="8" max="8" customWidth="true" width="9.42578125"/>
+    <col min="9" max="26" customWidth="true" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>70</v>
@@ -7793,19 +7858,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>45</v>
@@ -7819,19 +7884,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>52</v>
@@ -7845,25 +7910,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>80</v>
@@ -7871,19 +7936,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>45</v>
@@ -7897,22 +7962,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>55</v>
@@ -8909,65 +8974,67 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I999"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="52.28515625" customWidth="1"/>
-    <col min="10" max="26" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.42578125"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875"/>
+    <col min="3" max="3" customWidth="true" width="18.5703125"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125"/>
+    <col min="6" max="6" customWidth="true" width="8.5703125"/>
+    <col min="7" max="7" customWidth="true" width="9.85546875"/>
+    <col min="8" max="8" customWidth="true" width="13.28515625"/>
+    <col min="9" max="9" customWidth="true" width="52.28515625"/>
+    <col min="10" max="26" customWidth="true" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="E2" s="5">
         <v>45901.416666666664</v>
@@ -8976,74 +9043,44 @@
         <v>100</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D3" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E3" s="5">
+        <v>45935.583333333336</v>
+      </c>
+      <c r="F3" s="4">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10023,6 +10060,7 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>